<commit_message>
fixed fis summary tables
</commit_message>
<xml_diff>
--- a/region2017/reports/documents/FP/fishery_summary_table_formatted.xlsx
+++ b/region2017/reports/documents/FP/fishery_summary_table_formatted.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="740" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="-26640" yWindow="-720" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="fishery_summary_table" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +99,22 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,44 +154,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,211 +476,211 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="7" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11">
-        <v>41528.994791666599</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.79178745054052202</v>
+      <c r="C2" s="10">
+        <v>2392070.1</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.79223867475738596</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11">
-        <v>23299.535937500001</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.805927458230425</v>
+      <c r="C3" s="10">
+        <v>1192936.24</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.80595289430696104</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11">
-        <v>29654.5887362637</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.79598322446576197</v>
+      <c r="C4" s="10">
+        <v>2158854.06</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.79609520355579899</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="11">
-        <v>20028.225850340099</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.84716725700547701</v>
+      <c r="C5" s="10">
+        <v>588829.84</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0.84715068357022405</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="11">
-        <v>7085.8852459016398</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.87619307832422499</v>
+      <c r="C6" s="10">
+        <v>86447.8</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.87555555555555498</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="11">
-        <v>19263.1967213114</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.87568306010928898</v>
+      <c r="C7" s="10">
+        <v>235011</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.87555555555555498</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="11">
-        <v>4454.93103448275</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.87542145593869702</v>
+      <c r="C8" s="10">
+        <v>51677.2</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0.87555555555555498</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="11">
-        <v>4368.6825396825398</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.87580246913580195</v>
+      <c r="C9" s="10">
+        <v>55045.4</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0.87555555555555498</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="11">
-        <v>17013.063829787199</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C10" s="10">
+        <v>159922.79999999999</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="11">
-        <v>8513.2083333333303</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C11" s="10">
+        <v>81726.8</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="11">
-        <v>21991.184615384602</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="10">
+        <v>285885.40000000002</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="11">
-        <v>7301.9210526315701</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="C13" s="10">
+        <v>55494.6</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="12">
-        <v>1757561.2209302301</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.79804186046511605</v>
+        <v>30230053</v>
+      </c>
+      <c r="D14" s="13">
+        <v>0.79803516339869196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated pressure layers on sea level rise cc_slr_eco and cc_sealevel
</commit_message>
<xml_diff>
--- a/region2017/reports/documents/FP/fishery_summary_table_formatted.xlsx
+++ b/region2017/reports/documents/FP/fishery_summary_table_formatted.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28160" yWindow="-720" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="2440" yWindow="1260" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="fishery_summary_table" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="15">
   <si>
     <t>reef</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Mean Sustainability Score</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -558,7 +561,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -835,8 +838,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="17"/>
+      <c r="B22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="17">
+        <f>SUM(C18:C21)</f>
+        <v>33935905</v>
+      </c>
       <c r="D22" s="18"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>